<commit_message>
Add csv version of BOM
Easier access for GitHub
</commit_message>
<xml_diff>
--- a/Documentation/Working Documents/Open_Wobble_Switch_BOM.xlsx
+++ b/Documentation/Working Documents/Open_Wobble_Switch_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-RD/Shared Documents/20-11 RD Wobble Switch/8-Publishing/GitHub/Open-Wobble-Switch/Documentation/Working Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/Jake/Shared Documents/General/GitHub/Open-Wobble-Switch/Documentation/Working Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{2A6B6ED7-2222-48D6-9FEF-0D92DB627312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{713C1DEE-7FA9-487E-8E59-17E252FD33EB}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{2A6B6ED7-2222-48D6-9FEF-0D92DB627312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A61982A8-7E9F-43E8-A445-AB68FD2041F2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="116">
   <si>
     <t>Qty</t>
   </si>
@@ -297,12 +297,6 @@
     <t>OWS-111-001</t>
   </si>
   <si>
-    <t>Nameplate</t>
-  </si>
-  <si>
-    <t>Mounting Adapter</t>
-  </si>
-  <si>
     <t>OWS-100-001</t>
   </si>
   <si>
@@ -369,10 +363,28 @@
     <t>Optonal</t>
   </si>
   <si>
-    <t>Custom Topper Base</t>
-  </si>
-  <si>
     <t>Component name</t>
+  </si>
+  <si>
+    <t>Mounting Adapter (3D Printed)</t>
+  </si>
+  <si>
+    <t>Nameplate (3D Printed)</t>
+  </si>
+  <si>
+    <t>Topper Connector (3D Printed)</t>
+  </si>
+  <si>
+    <t>Topper Transition (3D Printed)</t>
+  </si>
+  <si>
+    <t>Topper Ball (3D Printed)</t>
+  </si>
+  <si>
+    <t>Topper Tee (3D Printed)</t>
+  </si>
+  <si>
+    <t>Custom Topper Base (3D Printed)</t>
   </si>
 </sst>
 </file>
@@ -380,7 +392,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -597,119 +609,107 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+  <cellXfs count="91">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="10" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="10" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="10" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="10" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="10" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="10" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="10" fillId="7" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="10" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="10" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="10" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="10" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="10" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="10" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="10" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
@@ -928,13 +928,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF999"/>
+  <dimension ref="A1:Q999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M35" sqref="M35"/>
+      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -949,1091 +949,994 @@
     <col min="8" max="8" width="15.875" style="9" customWidth="1"/>
     <col min="9" max="9" width="10.5" style="9" customWidth="1"/>
     <col min="10" max="10" width="3.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" style="51" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" style="45" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.25" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="7" style="51" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="7" style="45" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7" style="9" customWidth="1"/>
     <col min="17" max="17" width="108.125" style="9" bestFit="1" customWidth="1"/>
     <col min="18" max="32" width="7.625" style="9" customWidth="1"/>
     <col min="33" max="16384" width="12.625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="87" customFormat="1" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:17" s="77" customFormat="1" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="84" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="84" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="84" t="s">
+      <c r="C1" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="84" t="s">
+      <c r="F1" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="84" t="s">
+      <c r="G1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="84" t="s">
+      <c r="H1" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="84" t="s">
+      <c r="I1" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="85" t="s">
+      <c r="J1" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="86" t="s">
+      <c r="K1" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="85" t="s">
+      <c r="L1" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="86" t="s">
+      <c r="M1" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="86" t="s">
+      <c r="N1" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="86" t="s">
+      <c r="O1" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="84" t="s">
+      <c r="P1" s="75"/>
+      <c r="Q1" s="74" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="39" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+    <row r="2" spans="1:17" s="34" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="48">
+      <c r="K2" s="42"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="42">
         <f>SUM(M5:M21)</f>
         <v>82.33</v>
       </c>
-      <c r="N2" s="48"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="42">
+      <c r="N2" s="42"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="36">
         <f>SUM(O5:O17)</f>
         <v>15.060433333333334</v>
       </c>
     </row>
-    <row r="3" spans="1:32" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="43"/>
-    </row>
-    <row r="4" spans="1:32" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="43"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="37"/>
+    </row>
+    <row r="4" spans="1:17" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="13">
+      <c r="K4" s="44"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="12">
         <f>SUM(O5:O9)</f>
         <v>14.610533333333334</v>
       </c>
     </row>
-    <row r="5" spans="1:32" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="15">
-        <v>1</v>
-      </c>
-      <c r="C5" s="15" t="s">
+    <row r="5" spans="1:17" s="13" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="13">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="13">
         <v>3</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="15">
         <v>14.14</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="16">
         <f t="shared" ref="L5:L12" si="0">CEILING(B5/J5,1)</f>
         <v>1</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="15">
         <f>L5*K5</f>
         <v>14.14</v>
       </c>
-      <c r="N5" s="17">
+      <c r="N5" s="15">
         <f>K5/J5</f>
         <v>4.7133333333333338</v>
       </c>
-      <c r="O5" s="17">
+      <c r="O5" s="15">
         <f t="shared" ref="O5:O12" si="1">N5*B5</f>
         <v>4.7133333333333338</v>
       </c>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="19" t="s">
+      <c r="P5" s="15"/>
+      <c r="Q5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="15"/>
-    </row>
-    <row r="6" spans="1:32" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:17" s="13" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="15">
-        <v>1</v>
-      </c>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="13">
+        <v>1</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="13">
         <v>2</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6" s="15">
         <v>12.99</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="15">
         <f t="shared" ref="M6:M12" si="2">L6*K6</f>
         <v>12.99</v>
       </c>
-      <c r="N6" s="17">
+      <c r="N6" s="15">
         <f t="shared" ref="N6:N12" si="3">K6/J6</f>
         <v>6.4950000000000001</v>
       </c>
-      <c r="O6" s="17">
+      <c r="O6" s="15">
         <f t="shared" si="1"/>
         <v>6.4950000000000001</v>
       </c>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="19" t="s">
+      <c r="P6" s="15"/>
+      <c r="Q6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
-      <c r="AE6" s="15"/>
-      <c r="AF6" s="15"/>
-    </row>
-    <row r="7" spans="1:32" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:17" s="13" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="15">
-        <v>1</v>
-      </c>
-      <c r="C7" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="13">
         <v>100</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="15">
         <v>15.92</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="15">
         <f t="shared" si="2"/>
         <v>15.92</v>
       </c>
-      <c r="N7" s="17">
+      <c r="N7" s="15">
         <f t="shared" si="3"/>
         <v>0.15920000000000001</v>
       </c>
-      <c r="O7" s="17">
+      <c r="O7" s="15">
         <f t="shared" si="1"/>
         <v>0.15920000000000001</v>
       </c>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="19" t="s">
+      <c r="P7" s="15"/>
+      <c r="Q7" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:32" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="13" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="13">
         <v>4</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="21"/>
-      <c r="J8" s="14">
+      <c r="H8" s="19"/>
+      <c r="J8" s="13">
         <v>10</v>
       </c>
-      <c r="K8" s="22">
+      <c r="K8" s="20">
         <v>7.55</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="15">
         <f t="shared" si="2"/>
         <v>7.55</v>
       </c>
-      <c r="N8" s="17">
+      <c r="N8" s="15">
         <f t="shared" si="3"/>
         <v>0.755</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="15">
         <f t="shared" si="1"/>
         <v>3.02</v>
       </c>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="23" t="s">
+      <c r="P8" s="15"/>
+      <c r="Q8" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:32" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="13" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" s="15">
-        <v>1</v>
-      </c>
-      <c r="C9" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="13">
+        <v>1</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="13">
         <v>100</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="15">
         <v>22.3</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="15">
         <f t="shared" si="2"/>
         <v>22.3</v>
       </c>
-      <c r="N9" s="17">
+      <c r="N9" s="15">
         <f t="shared" si="3"/>
         <v>0.223</v>
       </c>
-      <c r="O9" s="17">
+      <c r="O9" s="15">
         <f t="shared" si="1"/>
         <v>0.223</v>
       </c>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="19" t="s">
+      <c r="P9" s="15"/>
+      <c r="Q9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
-      <c r="AA9" s="15"/>
-      <c r="AB9" s="15"/>
-      <c r="AC9" s="15"/>
-      <c r="AD9" s="15"/>
-      <c r="AE9" s="15"/>
-      <c r="AF9" s="15"/>
-    </row>
-    <row r="10" spans="1:32" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:17" s="13" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="15">
-        <v>1</v>
-      </c>
-      <c r="C10" s="14" t="s">
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15">
+      <c r="J10" s="13">
         <v>100</v>
       </c>
-      <c r="K10" s="17">
+      <c r="K10" s="15">
         <v>8.99</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M10" s="17">
+      <c r="M10" s="15">
         <f t="shared" si="2"/>
         <v>8.99</v>
       </c>
-      <c r="N10" s="17">
+      <c r="N10" s="15">
         <f t="shared" si="3"/>
         <v>8.9900000000000008E-2</v>
       </c>
-      <c r="O10" s="17">
+      <c r="O10" s="15">
         <f t="shared" si="1"/>
         <v>8.9900000000000008E-2</v>
       </c>
-      <c r="P10" s="15"/>
       <c r="Q10" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="15"/>
-      <c r="AB10" s="15"/>
-      <c r="AC10" s="15"/>
-      <c r="AD10" s="15"/>
-      <c r="AE10" s="15"/>
-      <c r="AF10" s="15"/>
-    </row>
-    <row r="11" spans="1:32" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="13" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="14">
-        <v>1</v>
-      </c>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="13">
+        <v>1</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="J11" s="14">
-        <v>1</v>
-      </c>
-      <c r="K11" s="22">
+      <c r="D11" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="J11" s="13">
+        <v>1</v>
+      </c>
+      <c r="K11" s="20">
         <v>0.2</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M11" s="17">
+      <c r="M11" s="15">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="N11" s="17">
+      <c r="N11" s="15">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="O11" s="17">
+      <c r="O11" s="15">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="Q11" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q11" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="13" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="14">
-        <v>1</v>
-      </c>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="13">
+        <v>1</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="J12" s="14">
-        <v>1</v>
-      </c>
-      <c r="K12" s="22">
+      <c r="D12" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="J12" s="13">
+        <v>1</v>
+      </c>
+      <c r="K12" s="20">
         <v>0.01</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="15">
         <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
-      <c r="N12" s="17">
+      <c r="N12" s="15">
         <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
-      <c r="O12" s="17">
+      <c r="O12" s="15">
         <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
-      <c r="Q12" s="19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" s="91" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="90" t="s">
+      <c r="Q12" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" s="13" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="91">
-        <v>1</v>
-      </c>
-      <c r="C13" s="91" t="s">
+      <c r="B13" s="13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="91" t="s">
-        <v>99</v>
-      </c>
-      <c r="J13" s="91">
-        <v>1</v>
-      </c>
-      <c r="K13" s="92">
+      <c r="D13" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="J13" s="13">
+        <v>1</v>
+      </c>
+      <c r="K13" s="80">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L13" s="93">
+      <c r="L13" s="81">
         <f>CEILING(B13/J13,1)</f>
         <v>1</v>
       </c>
-      <c r="M13" s="94">
+      <c r="M13" s="82">
         <f>L13*K13</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="N13" s="94">
+      <c r="N13" s="82">
         <f>K13/J13</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="O13" s="94">
+      <c r="O13" s="82">
         <f>N13*B13</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="Q13" s="95" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" s="24" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="24">
-        <v>1</v>
-      </c>
-      <c r="C14" s="24" t="s">
+      <c r="Q13" s="83" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" s="22" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="22">
+        <v>1</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="J14" s="24">
-        <v>1</v>
-      </c>
-      <c r="L14" s="24">
+      <c r="D14" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="J14" s="22">
+        <v>1</v>
+      </c>
+      <c r="L14" s="22">
         <f>CEILING(B14/J14,1)</f>
         <v>1</v>
       </c>
-      <c r="Q14" s="95" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Q15" s="25"/>
-    </row>
-    <row r="16" spans="1:32" s="26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q14" s="83" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q15" s="23"/>
+    </row>
+    <row r="16" spans="1:17" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="26">
-        <v>1</v>
-      </c>
-      <c r="C16" s="26" t="s">
+      <c r="B16" s="24">
+        <v>1</v>
+      </c>
+      <c r="C16" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="79" t="s">
+      <c r="D16" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="K16" s="52"/>
-      <c r="M16" s="52"/>
-      <c r="N16" s="52"/>
-      <c r="O16" s="52"/>
-      <c r="P16" s="26">
+      <c r="K16" s="46"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="46"/>
+      <c r="O16" s="46"/>
+      <c r="P16" s="24">
         <f>SUM(O17:O17)</f>
         <v>0.08</v>
       </c>
-      <c r="Q16" s="27"/>
-    </row>
-    <row r="17" spans="1:17" s="28" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q16" s="25"/>
+    </row>
+    <row r="17" spans="1:17" s="26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="28">
-        <v>1</v>
-      </c>
-      <c r="C17" s="28" t="s">
+      <c r="B17" s="26">
+        <v>1</v>
+      </c>
+      <c r="C17" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="J17" s="28">
-        <v>1</v>
-      </c>
-      <c r="K17" s="53">
+      <c r="D17" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="J17" s="26">
+        <v>1</v>
+      </c>
+      <c r="K17" s="47">
         <v>0.08</v>
       </c>
-      <c r="L17" s="29">
+      <c r="L17" s="27">
         <f>CEILING(B17/J17,1)</f>
         <v>1</v>
       </c>
-      <c r="M17" s="32">
+      <c r="M17" s="28">
         <f t="shared" ref="M17" si="4">L17*K17</f>
         <v>0.08</v>
       </c>
-      <c r="N17" s="32">
+      <c r="N17" s="28">
         <f t="shared" ref="N17" si="5">K17/J17</f>
         <v>0.08</v>
       </c>
-      <c r="O17" s="32">
+      <c r="O17" s="28">
         <f>N17*B17</f>
         <v>0.08</v>
       </c>
-      <c r="Q17" s="88" t="s">
-        <v>102</v>
+      <c r="Q17" s="78" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:17" s="33" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
+    <row r="19" spans="1:17" s="29" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="33">
-        <v>1</v>
-      </c>
-      <c r="C19" s="33" t="s">
+      <c r="B19" s="29">
+        <v>1</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="80" t="s">
+      <c r="D19" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="K19" s="54"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="54"/>
-      <c r="O19" s="54"/>
-      <c r="P19" s="33">
+      <c r="K19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="48"/>
+      <c r="P19" s="29">
         <f>SUM(O20:O20)</f>
         <v>0.08</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="34" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+    <row r="20" spans="1:17" s="30" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="34">
-        <v>1</v>
-      </c>
-      <c r="C20" s="34" t="s">
+      <c r="B20" s="30">
+        <v>1</v>
+      </c>
+      <c r="C20" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="J20" s="34">
-        <v>1</v>
-      </c>
-      <c r="K20" s="55">
+      <c r="D20" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="J20" s="30">
+        <v>1</v>
+      </c>
+      <c r="K20" s="49">
         <v>0.08</v>
       </c>
-      <c r="L20" s="35">
+      <c r="L20" s="31">
         <f>CEILING(B20/J20,1)</f>
         <v>1</v>
       </c>
-      <c r="M20" s="36">
+      <c r="M20" s="32">
         <f t="shared" ref="M20" si="6">L20*K20</f>
         <v>0.08</v>
       </c>
-      <c r="N20" s="36">
+      <c r="N20" s="32">
         <f t="shared" ref="N20" si="7">K20/J20</f>
         <v>0.08</v>
       </c>
-      <c r="O20" s="36">
+      <c r="O20" s="32">
         <f>N20*B20</f>
         <v>0.08</v>
       </c>
-      <c r="Q20" s="89" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-    </row>
-    <row r="22" spans="1:17" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="100" t="s">
-        <v>106</v>
-      </c>
-      <c r="B22" s="100">
-        <v>1</v>
-      </c>
-      <c r="C22" s="100" t="s">
+      <c r="Q20" s="79" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:17" s="88" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="88" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="88">
+        <v>1</v>
+      </c>
+      <c r="C22" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="101" t="s">
-        <v>107</v>
-      </c>
-      <c r="K22" s="102"/>
-      <c r="M22" s="102"/>
-      <c r="N22" s="102"/>
-      <c r="O22" s="102"/>
-      <c r="P22" s="33">
+      <c r="D22" s="89" t="s">
+        <v>105</v>
+      </c>
+      <c r="K22" s="90"/>
+      <c r="M22" s="90"/>
+      <c r="N22" s="90"/>
+      <c r="O22" s="90"/>
+      <c r="P22" s="29">
         <f>SUM(O23:O23)</f>
         <v>0.08</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="99" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="99" t="s">
-        <v>108</v>
-      </c>
-      <c r="B23" s="99">
-        <v>1</v>
-      </c>
-      <c r="C23" s="99" t="s">
-        <v>109</v>
-      </c>
-      <c r="D23" s="99" t="s">
-        <v>110</v>
-      </c>
-      <c r="J23" s="99">
-        <v>1</v>
-      </c>
-      <c r="K23" s="55">
+    <row r="23" spans="1:17" s="87" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="87">
+        <v>1</v>
+      </c>
+      <c r="C23" s="87" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="87" t="s">
+        <v>115</v>
+      </c>
+      <c r="J23" s="87">
+        <v>1</v>
+      </c>
+      <c r="K23" s="49">
         <v>0.08</v>
       </c>
-      <c r="L23" s="35">
+      <c r="L23" s="31">
         <f>CEILING(B23/J23,1)</f>
         <v>1</v>
       </c>
-      <c r="M23" s="36">
+      <c r="M23" s="32">
         <f t="shared" ref="M23" si="8">L23*K23</f>
         <v>0.08</v>
       </c>
-      <c r="N23" s="36">
+      <c r="N23" s="32">
         <f t="shared" ref="N23" si="9">K23/J23</f>
         <v>0.08</v>
       </c>
-      <c r="O23" s="36">
+      <c r="O23" s="32">
         <f>N23*B23</f>
         <v>0.08</v>
       </c>
-      <c r="Q23" s="89" t="s">
-        <v>103</v>
+      <c r="Q23" s="79" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:17" s="58" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="58" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" s="58">
+    <row r="25" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="9">
         <v>0</v>
       </c>
-      <c r="C25" s="59" t="s">
+      <c r="C25" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="60" t="s">
+      <c r="D25" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59" t="s">
+      <c r="F25" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J25" s="58">
+      <c r="J25" s="9">
         <v>2</v>
       </c>
-      <c r="K25" s="61">
+      <c r="K25" s="53">
         <v>14.93</v>
       </c>
-      <c r="L25" s="62">
+      <c r="L25" s="54">
         <f>CEILING(B25/J25,1)</f>
         <v>0</v>
       </c>
-      <c r="M25" s="63">
+      <c r="M25" s="55">
         <f t="shared" ref="M25:M26" si="10">L25*K25</f>
         <v>0</v>
       </c>
-      <c r="N25" s="63">
+      <c r="N25" s="55">
         <f>K25/J25</f>
         <v>7.4649999999999999</v>
       </c>
-      <c r="O25" s="63">
+      <c r="O25" s="55">
         <f>N25*B25</f>
         <v>0</v>
       </c>
-      <c r="P25" s="63"/>
-      <c r="Q25" s="64" t="s">
+      <c r="P25" s="55"/>
+      <c r="Q25" s="56" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="58" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="58" t="s">
-        <v>88</v>
-      </c>
-      <c r="B26" s="58">
+    <row r="26" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="9">
         <v>0</v>
       </c>
-      <c r="C26" s="59" t="s">
+      <c r="C26" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="60" t="s">
+      <c r="D26" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59" t="s">
+      <c r="F26" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J26" s="58">
+      <c r="J26" s="9">
         <v>3</v>
       </c>
-      <c r="K26" s="61">
+      <c r="K26" s="53">
         <f>14.14+5.59</f>
         <v>19.73</v>
       </c>
-      <c r="L26" s="62">
+      <c r="L26" s="54">
         <f>CEILING(B26/J26,1)</f>
         <v>0</v>
       </c>
-      <c r="M26" s="63">
+      <c r="M26" s="55">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="N26" s="63">
+      <c r="N26" s="55">
         <f>K26/J26</f>
         <v>6.5766666666666671</v>
       </c>
-      <c r="O26" s="63">
+      <c r="O26" s="55">
         <f>N26*B26</f>
         <v>0</v>
       </c>
-      <c r="P26" s="63"/>
-      <c r="Q26" s="64" t="s">
+      <c r="P26" s="55"/>
+      <c r="Q26" s="56" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="58" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="58" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27" s="58">
+    <row r="27" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="9">
         <v>0</v>
       </c>
-      <c r="C27" s="59" t="s">
+      <c r="C27" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="60" t="s">
+      <c r="D27" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59" t="s">
+      <c r="F27" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J27" s="58">
-        <v>1</v>
-      </c>
-      <c r="K27" s="61">
+      <c r="J27" s="9">
+        <v>1</v>
+      </c>
+      <c r="K27" s="53">
         <v>14.19</v>
       </c>
-      <c r="L27" s="62">
+      <c r="L27" s="54">
         <f>CEILING(B27/J27,1)</f>
         <v>0</v>
       </c>
-      <c r="M27" s="63">
+      <c r="M27" s="55">
         <f t="shared" ref="M27" si="11">L27*K27</f>
         <v>0</v>
       </c>
-      <c r="N27" s="63">
+      <c r="N27" s="55">
         <f>K27/J27</f>
         <v>14.19</v>
       </c>
-      <c r="O27" s="63">
+      <c r="O27" s="55">
         <f>N27*B27</f>
         <v>0</v>
       </c>
-      <c r="P27" s="63"/>
-      <c r="Q27" s="64" t="s">
+      <c r="P27" s="55"/>
+      <c r="Q27" s="56" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="58" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="59"/>
-      <c r="K28" s="61"/>
-      <c r="M28" s="61"/>
-      <c r="N28" s="61"/>
-      <c r="O28" s="61"/>
-      <c r="Q28" s="65"/>
-    </row>
-    <row r="29" spans="1:17" s="58" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="53"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="53"/>
+      <c r="O28" s="53"/>
+      <c r="Q28" s="23"/>
+    </row>
+    <row r="29" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="59">
+        <v>91</v>
+      </c>
+      <c r="B29" s="9">
         <v>0</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="60" t="s">
+      <c r="D29" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59" t="s">
+      <c r="F29" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59">
-        <v>1</v>
-      </c>
-      <c r="K29" s="63">
+      <c r="J29" s="9">
+        <v>1</v>
+      </c>
+      <c r="K29" s="55">
         <v>0.24</v>
       </c>
-      <c r="L29" s="62">
+      <c r="L29" s="54">
         <f>CEILING(B29/J29,1)</f>
         <v>0</v>
       </c>
-      <c r="M29" s="63">
+      <c r="M29" s="55">
         <f t="shared" ref="M29:M30" si="12">L29*K29</f>
         <v>0</v>
       </c>
-      <c r="N29" s="63">
+      <c r="N29" s="55">
         <f t="shared" ref="N29:N30" si="13">K29/J29</f>
         <v>0.24</v>
       </c>
-      <c r="O29" s="63">
+      <c r="O29" s="55">
         <f>N29*B29</f>
         <v>0</v>
       </c>
-      <c r="P29" s="63"/>
-      <c r="Q29" s="67" t="s">
+      <c r="P29" s="55"/>
+      <c r="Q29" s="58" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" s="58" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B30" s="59">
+      <c r="B30" s="9">
         <v>0</v>
       </c>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="66" t="s">
+      <c r="D30" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="59" t="s">
+      <c r="F30" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G30" s="59"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="59">
-        <v>1</v>
-      </c>
-      <c r="K30" s="63">
+      <c r="J30" s="9">
+        <v>1</v>
+      </c>
+      <c r="K30" s="55">
         <v>0.48</v>
       </c>
-      <c r="L30" s="62">
+      <c r="L30" s="54">
         <f>CEILING(B30/J30,1)</f>
         <v>0</v>
       </c>
-      <c r="M30" s="63">
+      <c r="M30" s="55">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="N30" s="63">
+      <c r="N30" s="55">
         <f t="shared" si="13"/>
         <v>0.48</v>
       </c>
-      <c r="O30" s="63">
+      <c r="O30" s="55">
         <f>N30*B30</f>
         <v>0</v>
       </c>
-      <c r="P30" s="63"/>
-      <c r="Q30" s="67" t="s">
-        <v>90</v>
+      <c r="P30" s="55"/>
+      <c r="Q30" s="58" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="31"/>
-      <c r="Q31" s="25"/>
+      <c r="Q31" s="23"/>
     </row>
     <row r="32" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="31"/>
-      <c r="Q32" s="25"/>
-    </row>
-    <row r="33" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="31"/>
-      <c r="Q33" s="25"/>
-    </row>
-    <row r="34" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="31"/>
-      <c r="Q34" s="25"/>
-    </row>
-    <row r="35" spans="3:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="31"/>
-      <c r="Q35" s="25"/>
-    </row>
-    <row r="36" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="31"/>
-    </row>
-    <row r="37" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Q37" s="25"/>
-    </row>
-    <row r="38" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Q39" s="25"/>
-    </row>
-    <row r="40" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="3:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="Q32" s="23"/>
+    </row>
+    <row r="33" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q33" s="23"/>
+    </row>
+    <row r="34" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q34" s="23"/>
+    </row>
+    <row r="35" spans="17:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q35" s="23"/>
+    </row>
+    <row r="36" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q37" s="23"/>
+    </row>
+    <row r="38" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q39" s="23"/>
+    </row>
+    <row r="40" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="17:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3028,7 +2931,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="38" t="s">
         <v>67</v>
       </c>
       <c r="B1" s="2"/>
@@ -3038,72 +2941,72 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="39" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45">
-        <v>1</v>
-      </c>
-      <c r="F3" s="45"/>
-    </row>
-    <row r="4" spans="1:6" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="77" t="s">
+      <c r="D3" s="39"/>
+      <c r="E3" s="39">
+        <v>1</v>
+      </c>
+      <c r="F3" s="39"/>
+    </row>
+    <row r="4" spans="1:6" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77">
-        <v>1</v>
-      </c>
-      <c r="F4" s="77"/>
-    </row>
-    <row r="5" spans="1:6" s="78" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="77" t="s">
+      <c r="D4" s="68"/>
+      <c r="E4" s="68">
+        <v>1</v>
+      </c>
+      <c r="F4" s="68"/>
+    </row>
+    <row r="5" spans="1:6" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77">
-        <v>1</v>
-      </c>
-      <c r="F5" s="77"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68">
+        <v>1</v>
+      </c>
+      <c r="F5" s="68"/>
     </row>
     <row r="6" spans="1:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -3180,7 +3083,7 @@
         <v>85</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>54</v>
@@ -3195,7 +3098,7 @@
     </row>
     <row r="11" spans="1:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>70</v>
@@ -3231,9 +3134,9 @@
     </row>
     <row r="13" spans="1:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -3269,8 +3172,8 @@
       <c r="A15" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="96" t="s">
-        <v>99</v>
+      <c r="B15" s="84" t="s">
+        <v>97</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>54</v>
@@ -3284,16 +3187,16 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="96" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="96" t="s">
-        <v>101</v>
-      </c>
-      <c r="C16" s="96" t="s">
+      <c r="A16" s="84" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="84" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="96" t="s">
+      <c r="D16" s="84" t="s">
         <v>58</v>
       </c>
       <c r="E16" s="8">
@@ -3317,28 +3220,28 @@
       </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" s="76" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="75" t="s">
+    <row r="18" spans="1:6" s="67" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="75" t="s">
+      <c r="C18" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75">
-        <v>1</v>
-      </c>
-      <c r="F18" s="75"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66">
+        <v>1</v>
+      </c>
+      <c r="F18" s="66"/>
     </row>
     <row r="19" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="97" t="s">
-        <v>97</v>
+      <c r="B19" s="85" t="s">
+        <v>95</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>54</v>
@@ -3351,81 +3254,81 @@
       </c>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" s="73" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="72" t="s">
+    <row r="20" spans="1:6" s="64" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="72" t="s">
+      <c r="C20" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72">
-        <v>1</v>
-      </c>
-      <c r="F20" s="72"/>
-    </row>
-    <row r="21" spans="1:6" s="74" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
+      <c r="D20" s="63"/>
+      <c r="E20" s="63">
+        <v>1</v>
+      </c>
+      <c r="F20" s="63"/>
+    </row>
+    <row r="21" spans="1:6" s="65" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="98" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="46" t="s">
+      <c r="B21" s="86" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="46">
-        <v>1</v>
-      </c>
-      <c r="F21" s="46"/>
-    </row>
-    <row r="22" spans="1:6" s="74" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
-      <c r="B22" s="98"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-    </row>
-    <row r="23" spans="1:6" s="71" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="70" t="s">
+      <c r="E21" s="40">
+        <v>1</v>
+      </c>
+      <c r="F21" s="40"/>
+    </row>
+    <row r="22" spans="1:6" s="65" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="40"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+    </row>
+    <row r="23" spans="1:6" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="70" t="s">
+      <c r="B23" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="70" t="s">
+      <c r="C23" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70">
-        <v>1</v>
-      </c>
-      <c r="F23" s="70"/>
-    </row>
-    <row r="24" spans="1:6" s="69" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="68" t="s">
+      <c r="D23" s="61"/>
+      <c r="E23" s="61">
+        <v>1</v>
+      </c>
+      <c r="F23" s="61"/>
+    </row>
+    <row r="24" spans="1:6" s="60" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="68" t="s">
+      <c r="C24" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="68" t="s">
+      <c r="D24" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="68">
-        <v>1</v>
-      </c>
-      <c r="F24" s="68"/>
+      <c r="E24" s="59">
+        <v>1</v>
+      </c>
+      <c r="F24" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3442,16 +3345,10 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B51EC7ECFAC78D4E8EF6CBAFFF0B3505" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c1c974e075ae6ad637ed0c9d0de986aa">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e" xmlns:ns3="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6f8b78299b17ebfa6252ff38db7b045f" ns2:_="" ns3:_="">
-    <xsd:import namespace="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
-    <xsd:import namespace="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001DC44D19606E8540AF995795CBBBCE63" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="72518c49cc9021390dbba2958e7a3f0c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e718a8af-5d48-45b1-a7fb-cef00c107a7a" xmlns:ns3="715913e6-4bf0-458f-8160-f18e142d04ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="175092e7cad6d6b91dac7c2ca96d6cf8" ns2:_="" ns3:_="">
+    <xsd:import namespace="e718a8af-5d48-45b1-a7fb-cef00c107a7a"/>
+    <xsd:import namespace="715913e6-4bf0-458f-8160-f18e142d04ff"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -3462,14 +3359,16 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3477,7 +3376,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e718a8af-5d48-45b1-a7fb-cef00c107a7a" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -3502,31 +3401,31 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+    <xsd:element name="MediaLengthInSeconds" ma:index="16" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
@@ -3534,35 +3433,37 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="26ec1fed-e6ae-4c84-a4ac-123136fd9316" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="21" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="715913e6-4bf0-458f-8160-f18e142d04ff" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="TaxCatchAll" ma:index="20" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{b05470fb-f248-421d-a4ae-c1bb0b45488d}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="715913e6-4bf0-458f-8160-f18e142d04ff">
       <xsd:complexType>
         <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
+          <xsd:extension base="dms:MultiChoiceLookup">
             <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
             </xsd:sequence>
           </xsd:extension>
         </xsd:complexContent>
       </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -3664,6 +3565,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="715913e6-4bf0-458f-8160-f18e142d04ff" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e718a8af-5d48-45b1-a7fb-cef00c107a7a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57B67867-0919-40B4-9C97-1BEA0F6DE45E}">
   <ds:schemaRefs>
@@ -3673,6 +3585,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E7CD765-31AD-47C8-BF28-7DC39AB6B632}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e718a8af-5d48-45b1-a7fb-cef00c107a7a"/>
+    <ds:schemaRef ds:uri="715913e6-4bf0-458f-8160-f18e142d04ff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{026AE4C7-CA26-46A3-AA6B-5C77B6D4BCB6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
@@ -3685,25 +3616,8 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0414048A-9692-4AD5-AD94-5756C37A95C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
-    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="715913e6-4bf0-458f-8160-f18e142d04ff"/>
+    <ds:schemaRef ds:uri="e718a8af-5d48-45b1-a7fb-cef00c107a7a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>